<commit_message>
Suppord for a permanent extraDownpayment schedule to mrotgage, reducing the lengt of the mortgage
</commit_message>
<xml_diff>
--- a/tests/Feature/config/mortgage_zero.xlsx
+++ b/tests/Feature/config/mortgage_zero.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>private</t>
   </si>
@@ -166,8 +166,11 @@
     <t xml:space="preserve"> Asset rule: </t>
   </si>
   <si>
-    <t xml:space="preserve"> Asset rule: Using current amount: 3000000 * 1 extraDownpaymentAmount: 60000
+    <t xml:space="preserve"> Asset rule: Using current amount: 3000000 * 1 extraDownpaymentAmount: 150000
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Asset rule: Using current amount: 3000000 * 1Mortgage payed 4 years faster due to extraDownpayments</t>
   </si>
   <si>
     <t xml:space="preserve"> Asset rule: Using current amount: 3000000 * 1</t>
@@ -1869,10 +1872,10 @@
         <v>15000.0</v>
       </c>
       <c r="L18" s="1">
-        <v>203373.0</v>
+        <v>293373.0</v>
       </c>
       <c r="M18" s="1">
-        <v>1296627.0</v>
+        <v>1206627.0</v>
       </c>
       <c r="N18" s="1">
         <v>0</v>
@@ -1883,7 +1886,7 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="1">
-        <v>1703373.0</v>
+        <v>1793373.0</v>
       </c>
       <c r="S18" s="1">
         <v>3000000.0</v>
@@ -1949,17 +1952,17 @@
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="8">
-        <v>151369.0</v>
+        <v>140862.0</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="8">
-        <v>12966.0</v>
+        <v>12066.0</v>
       </c>
       <c r="L19" s="8">
-        <v>198402.0</v>
+        <v>278796.0</v>
       </c>
       <c r="M19" s="8">
-        <v>1098224.0</v>
+        <v>927831.0</v>
       </c>
       <c r="N19" s="8">
         <v>0</v>
@@ -1970,13 +1973,13 @@
       </c>
       <c r="Q19" s="9"/>
       <c r="R19" s="8">
-        <v>1901776.0</v>
+        <v>2072169.0</v>
       </c>
       <c r="S19" s="8">
         <v>3000000.0</v>
       </c>
       <c r="T19" s="8">
-        <v>1651369.0</v>
+        <v>1640862.0</v>
       </c>
       <c r="U19" s="8">
         <v>750000.0</v>
@@ -1997,20 +2000,20 @@
       </c>
       <c r="AD19" s="9"/>
       <c r="AE19" s="8">
-        <v>-155569.0</v>
+        <v>-145062.0</v>
       </c>
       <c r="AF19" s="8">
-        <v>-318142.0</v>
+        <v>-307635.0</v>
       </c>
       <c r="AG19" s="9"/>
       <c r="AH19" s="8">
-        <v>-151369.0</v>
+        <v>-140862.0</v>
       </c>
       <c r="AI19" s="8">
-        <v>-756845.0</v>
+        <v>-704310.0</v>
       </c>
       <c r="AJ19" s="8">
-        <v>-12966.0</v>
+        <v>-12066.0</v>
       </c>
       <c r="AK19" s="8"/>
       <c r="AL19" s="9"/>
@@ -2036,17 +2039,17 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1">
-        <v>143527.0</v>
+        <v>121259.0</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="1">
-        <v>10982.0</v>
+        <v>9278.0</v>
       </c>
       <c r="L20" s="1">
-        <v>192545.0</v>
+        <v>261980.0</v>
       </c>
       <c r="M20" s="1">
-        <v>905679.0</v>
+        <v>665851.0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -2057,13 +2060,13 @@
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>2094321.0</v>
+        <v>2334149.0</v>
       </c>
       <c r="S20" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T20" s="1">
-        <v>1794896.0</v>
+        <v>1762121.0</v>
       </c>
       <c r="U20" s="6">
         <v>750000.0</v>
@@ -2084,20 +2087,20 @@
       </c>
       <c r="AD20" s="2"/>
       <c r="AE20" s="1">
-        <v>-147727.0</v>
+        <v>-125459.0</v>
       </c>
       <c r="AF20" s="1">
-        <v>-465869.0</v>
+        <v>-433094.0</v>
       </c>
       <c r="AG20" s="2"/>
       <c r="AH20" s="1">
-        <v>-143527.0</v>
+        <v>-121259.0</v>
       </c>
       <c r="AI20" s="1">
-        <v>-717635.0</v>
+        <v>-606295.0</v>
       </c>
       <c r="AJ20" s="1">
-        <v>-10982.0</v>
+        <v>-9278.0</v>
       </c>
       <c r="AK20" s="1"/>
       <c r="AL20" s="2"/>
@@ -2123,17 +2126,17 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1">
-        <v>134610.0</v>
+        <v>98964.0</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="1">
-        <v>9057.0</v>
+        <v>6659.0</v>
       </c>
       <c r="L21" s="1">
-        <v>185553.0</v>
+        <v>242306.0</v>
       </c>
       <c r="M21" s="1">
-        <v>720127.0</v>
+        <v>423545.0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
@@ -2144,13 +2147,13 @@
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="1">
-        <v>2279873.0</v>
+        <v>2576455.0</v>
       </c>
       <c r="S21" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T21" s="1">
-        <v>1929506.0</v>
+        <v>1861085.0</v>
       </c>
       <c r="U21" s="6">
         <v>750000.0</v>
@@ -2171,20 +2174,20 @@
       </c>
       <c r="AD21" s="2"/>
       <c r="AE21" s="1">
-        <v>-138810.0</v>
+        <v>-103164.0</v>
       </c>
       <c r="AF21" s="1">
-        <v>-604679.0</v>
+        <v>-536258.0</v>
       </c>
       <c r="AG21" s="2"/>
       <c r="AH21" s="1">
-        <v>-134610.0</v>
+        <v>-98964.0</v>
       </c>
       <c r="AI21" s="1">
-        <v>-673050.0</v>
+        <v>-494820.0</v>
       </c>
       <c r="AJ21" s="1">
-        <v>-9057.0</v>
+        <v>-6659.0</v>
       </c>
       <c r="AK21" s="1"/>
       <c r="AL21" s="2"/>
@@ -2210,17 +2213,17 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1">
-        <v>124257.0</v>
+        <v>73082.0</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="1">
-        <v>7201.0</v>
+        <v>4235.0</v>
       </c>
       <c r="L22" s="1">
-        <v>177055.0</v>
+        <v>218847.0</v>
       </c>
       <c r="M22" s="1">
-        <v>543071.0</v>
+        <v>204699.0</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
@@ -2231,13 +2234,13 @@
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="1">
-        <v>2456929.0</v>
+        <v>2795301.0</v>
       </c>
       <c r="S22" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T22" s="1">
-        <v>2053763.0</v>
+        <v>1934167.0</v>
       </c>
       <c r="U22" s="6">
         <v>750000.0</v>
@@ -2258,20 +2261,20 @@
       </c>
       <c r="AD22" s="2"/>
       <c r="AE22" s="1">
-        <v>-128457.0</v>
+        <v>-77282.0</v>
       </c>
       <c r="AF22" s="1">
-        <v>-733136.0</v>
+        <v>-613540.0</v>
       </c>
       <c r="AG22" s="2"/>
       <c r="AH22" s="1">
-        <v>-124257.0</v>
+        <v>-73082.0</v>
       </c>
       <c r="AI22" s="1">
-        <v>-621285.0</v>
+        <v>-365410.0</v>
       </c>
       <c r="AJ22" s="1">
-        <v>-7201.0</v>
+        <v>-4235.0</v>
       </c>
       <c r="AK22" s="1"/>
       <c r="AL22" s="2"/>
@@ -2297,17 +2300,17 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1">
-        <v>111894.0</v>
+        <v>42176.0</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="1">
-        <v>5431.0</v>
+        <v>2047.0</v>
       </c>
       <c r="L23" s="1">
-        <v>166464.0</v>
+        <v>190129.0</v>
       </c>
       <c r="M23" s="1">
-        <v>376608.0</v>
+        <v>14569.0</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -2318,13 +2321,13 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="1">
-        <v>2623392.0</v>
+        <v>2985431.0</v>
       </c>
       <c r="S23" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T23" s="1">
-        <v>2165657.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U23" s="6">
         <v>750000.0</v>
@@ -2345,20 +2348,20 @@
       </c>
       <c r="AD23" s="2"/>
       <c r="AE23" s="1">
-        <v>-116094.0</v>
+        <v>-46376.0</v>
       </c>
       <c r="AF23" s="1">
-        <v>-849230.0</v>
+        <v>-659916.0</v>
       </c>
       <c r="AG23" s="2"/>
       <c r="AH23" s="1">
-        <v>-111894.0</v>
+        <v>-42176.0</v>
       </c>
       <c r="AI23" s="1">
-        <v>-559470.0</v>
+        <v>-210880.0</v>
       </c>
       <c r="AJ23" s="1">
-        <v>-5431.0</v>
+        <v>-2047.0</v>
       </c>
       <c r="AK23" s="1"/>
       <c r="AL23" s="2"/>
@@ -2384,17 +2387,17 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1">
-        <v>96517.0</v>
+        <v>0</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="1">
-        <v>3766.0</v>
+        <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>152751.0</v>
+        <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>223856.0</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -2405,13 +2408,13 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="1">
-        <v>2776144.0</v>
+        <v>3000000.0</v>
       </c>
       <c r="S24" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T24" s="1">
-        <v>2262174.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U24" s="6">
         <v>750000.0</v>
@@ -2432,20 +2435,20 @@
       </c>
       <c r="AD24" s="2"/>
       <c r="AE24" s="1">
-        <v>-100717.0</v>
+        <v>-4200.0</v>
       </c>
       <c r="AF24" s="1">
-        <v>-949947.0</v>
+        <v>-664116.0</v>
       </c>
       <c r="AG24" s="2"/>
       <c r="AH24" s="1">
-        <v>-96517.0</v>
+        <v>0.0</v>
       </c>
       <c r="AI24" s="1">
-        <v>-482585.0</v>
+        <v>0.0</v>
       </c>
       <c r="AJ24" s="1">
-        <v>-3766.0</v>
+        <v>0.0</v>
       </c>
       <c r="AK24" s="1"/>
       <c r="AL24" s="2"/>
@@ -2471,17 +2474,17 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1">
-        <v>76116.0</v>
+        <v>0</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="1">
-        <v>2239.0</v>
+        <v>0</v>
       </c>
       <c r="L25" s="1">
-        <v>133878.0</v>
+        <v>0</v>
       </c>
       <c r="M25" s="1">
-        <v>89979.0</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1">
         <v>0</v>
@@ -2492,13 +2495,13 @@
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="1">
-        <v>2910021.0</v>
+        <v>3000000.0</v>
       </c>
       <c r="S25" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T25" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U25" s="6">
         <v>750000.0</v>
@@ -2519,20 +2522,20 @@
       </c>
       <c r="AD25" s="2"/>
       <c r="AE25" s="1">
-        <v>-80316.0</v>
+        <v>-4200.0</v>
       </c>
       <c r="AF25" s="1">
-        <v>-1030263.0</v>
+        <v>-668316.0</v>
       </c>
       <c r="AG25" s="2"/>
       <c r="AH25" s="1">
-        <v>-76116.0</v>
+        <v>0.0</v>
       </c>
       <c r="AI25" s="1">
-        <v>-380580.0</v>
+        <v>0.0</v>
       </c>
       <c r="AJ25" s="1">
-        <v>-2239.0</v>
+        <v>0.0</v>
       </c>
       <c r="AK25" s="1"/>
       <c r="AL25" s="2"/>
@@ -2585,7 +2588,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T26" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U26" s="6">
         <v>750000.0</v>
@@ -2609,7 +2612,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF26" s="1">
-        <v>-1034463.0</v>
+        <v>-672516.0</v>
       </c>
       <c r="AG26" s="2"/>
       <c r="AH26" s="1">
@@ -2672,7 +2675,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T27" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U27" s="6">
         <v>750000.0</v>
@@ -2696,7 +2699,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF27" s="1">
-        <v>-1038663.0</v>
+        <v>-676716.0</v>
       </c>
       <c r="AG27" s="2"/>
       <c r="AH27" s="1">
@@ -2759,7 +2762,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T28" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U28" s="6">
         <v>750000.0</v>
@@ -2783,7 +2786,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF28" s="1">
-        <v>-1042863.0</v>
+        <v>-680916.0</v>
       </c>
       <c r="AG28" s="2"/>
       <c r="AH28" s="1">
@@ -2846,7 +2849,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T29" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U29" s="6">
         <v>750000.0</v>
@@ -2870,7 +2873,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF29" s="1">
-        <v>-1047063.0</v>
+        <v>-685116.0</v>
       </c>
       <c r="AG29" s="2"/>
       <c r="AH29" s="1">
@@ -2933,7 +2936,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T30" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U30" s="6">
         <v>750000.0</v>
@@ -2957,7 +2960,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF30" s="1">
-        <v>-1051263.0</v>
+        <v>-689316.0</v>
       </c>
       <c r="AG30" s="2"/>
       <c r="AH30" s="1">
@@ -3020,7 +3023,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T31" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U31" s="6">
         <v>750000.0</v>
@@ -3044,7 +3047,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF31" s="1">
-        <v>-1055463.0</v>
+        <v>-693516.0</v>
       </c>
       <c r="AG31" s="2"/>
       <c r="AH31" s="1">
@@ -3107,7 +3110,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T32" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U32" s="6">
         <v>750000.0</v>
@@ -3131,7 +3134,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF32" s="1">
-        <v>-1059663.0</v>
+        <v>-697716.0</v>
       </c>
       <c r="AG32" s="2"/>
       <c r="AH32" s="1">
@@ -3194,7 +3197,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T33" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U33" s="6">
         <v>750000.0</v>
@@ -3218,7 +3221,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF33" s="1">
-        <v>-1063863.0</v>
+        <v>-701916.0</v>
       </c>
       <c r="AG33" s="2"/>
       <c r="AH33" s="1">
@@ -3281,7 +3284,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T34" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U34" s="6">
         <v>750000.0</v>
@@ -3305,7 +3308,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF34" s="1">
-        <v>-1068063.0</v>
+        <v>-706116.0</v>
       </c>
       <c r="AG34" s="2"/>
       <c r="AH34" s="1">
@@ -3368,7 +3371,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T35" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U35" s="6">
         <v>750000.0</v>
@@ -3392,7 +3395,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF35" s="1">
-        <v>-1072263.0</v>
+        <v>-710316.0</v>
       </c>
       <c r="AG35" s="2"/>
       <c r="AH35" s="1">
@@ -3455,7 +3458,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T36" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U36" s="6">
         <v>750000.0</v>
@@ -3479,7 +3482,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF36" s="1">
-        <v>-1076463.0</v>
+        <v>-714516.0</v>
       </c>
       <c r="AG36" s="2"/>
       <c r="AH36" s="1">
@@ -3542,7 +3545,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T37" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U37" s="6">
         <v>750000.0</v>
@@ -3566,7 +3569,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF37" s="1">
-        <v>-1080663.0</v>
+        <v>-718716.0</v>
       </c>
       <c r="AG37" s="2"/>
       <c r="AH37" s="1">
@@ -3629,7 +3632,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T38" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U38" s="6">
         <v>750000.0</v>
@@ -3653,7 +3656,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF38" s="1">
-        <v>-1084863.0</v>
+        <v>-722916.0</v>
       </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1">
@@ -3716,7 +3719,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T39" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U39" s="6">
         <v>750000.0</v>
@@ -3740,7 +3743,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF39" s="1">
-        <v>-1089063.0</v>
+        <v>-727116.0</v>
       </c>
       <c r="AG39" s="2"/>
       <c r="AH39" s="1">
@@ -3803,7 +3806,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T40" s="11">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U40" s="11">
         <v>750000.0</v>
@@ -3827,7 +3830,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF40" s="11">
-        <v>-1093263.0</v>
+        <v>-731316.0</v>
       </c>
       <c r="AG40" s="12"/>
       <c r="AH40" s="11">
@@ -3890,7 +3893,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T41" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U41" s="6">
         <v>750000.0</v>
@@ -3914,7 +3917,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF41" s="1">
-        <v>-1097463.0</v>
+        <v>-735516.0</v>
       </c>
       <c r="AG41" s="2"/>
       <c r="AH41" s="1">
@@ -3977,7 +3980,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T42" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U42" s="6">
         <v>750000.0</v>
@@ -4001,7 +4004,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF42" s="1">
-        <v>-1101663.0</v>
+        <v>-739716.0</v>
       </c>
       <c r="AG42" s="2"/>
       <c r="AH42" s="1">
@@ -4064,7 +4067,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T43" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U43" s="6">
         <v>750000.0</v>
@@ -4088,7 +4091,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF43" s="1">
-        <v>-1105863.0</v>
+        <v>-743916.0</v>
       </c>
       <c r="AG43" s="2"/>
       <c r="AH43" s="1">
@@ -4151,7 +4154,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T44" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U44" s="6">
         <v>750000.0</v>
@@ -4175,7 +4178,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF44" s="1">
-        <v>-1110063.0</v>
+        <v>-748116.0</v>
       </c>
       <c r="AG44" s="2"/>
       <c r="AH44" s="1">
@@ -4238,7 +4241,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T45" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U45" s="6">
         <v>750000.0</v>
@@ -4262,7 +4265,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF45" s="1">
-        <v>-1114263.0</v>
+        <v>-752316.0</v>
       </c>
       <c r="AG45" s="2"/>
       <c r="AH45" s="1">
@@ -4325,7 +4328,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T46" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U46" s="6">
         <v>750000.0</v>
@@ -4349,7 +4352,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF46" s="1">
-        <v>-1118463.0</v>
+        <v>-756516.0</v>
       </c>
       <c r="AG46" s="2"/>
       <c r="AH46" s="1">
@@ -4412,7 +4415,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T47" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U47" s="6">
         <v>750000.0</v>
@@ -4436,7 +4439,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF47" s="1">
-        <v>-1122663.0</v>
+        <v>-760716.0</v>
       </c>
       <c r="AG47" s="2"/>
       <c r="AH47" s="1">
@@ -4499,7 +4502,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T48" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U48" s="6">
         <v>750000.0</v>
@@ -4523,7 +4526,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF48" s="1">
-        <v>-1126863.0</v>
+        <v>-764916.0</v>
       </c>
       <c r="AG48" s="2"/>
       <c r="AH48" s="1">
@@ -4586,7 +4589,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T49" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U49" s="6">
         <v>750000.0</v>
@@ -4610,7 +4613,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF49" s="1">
-        <v>-1131063.0</v>
+        <v>-769116.0</v>
       </c>
       <c r="AG49" s="2"/>
       <c r="AH49" s="1">
@@ -4673,7 +4676,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T50" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U50" s="6">
         <v>750000.0</v>
@@ -4697,7 +4700,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF50" s="1">
-        <v>-1135263.0</v>
+        <v>-773316.0</v>
       </c>
       <c r="AG50" s="2"/>
       <c r="AH50" s="1">
@@ -4760,7 +4763,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T51" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U51" s="6">
         <v>750000.0</v>
@@ -4784,7 +4787,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF51" s="1">
-        <v>-1139463.0</v>
+        <v>-777516.0</v>
       </c>
       <c r="AG51" s="2"/>
       <c r="AH51" s="1">
@@ -4847,7 +4850,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T52" s="5">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U52" s="5">
         <v>750000.0</v>
@@ -4871,7 +4874,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF52" s="5">
-        <v>-1143663.0</v>
+        <v>-781716.0</v>
       </c>
       <c r="AG52" s="16"/>
       <c r="AH52" s="5">
@@ -7263,10 +7266,10 @@
         <v>15000.0</v>
       </c>
       <c r="L18" s="1">
-        <v>203373.0</v>
+        <v>293373.0</v>
       </c>
       <c r="M18" s="1">
-        <v>1296627.0</v>
+        <v>1206627.0</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="2"/>
@@ -7275,7 +7278,7 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="1">
-        <v>1703373.0</v>
+        <v>1793373.0</v>
       </c>
       <c r="S18" s="1">
         <v>3000000.0</v>
@@ -7318,7 +7321,7 @@
         <v>-162573.0</v>
       </c>
       <c r="AG18" s="2">
-        <v>0.432209</v>
+        <v>0.402209</v>
       </c>
       <c r="AH18" s="1">
         <v>-158373.0</v>
@@ -7357,19 +7360,19 @@
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="8">
-        <v>151369.0</v>
+        <v>140862.0</v>
       </c>
       <c r="J19" s="9">
         <v>0.01</v>
       </c>
       <c r="K19" s="8">
-        <v>12966.0</v>
+        <v>12066.0</v>
       </c>
       <c r="L19" s="8">
-        <v>198402.0</v>
+        <v>278796.0</v>
       </c>
       <c r="M19" s="8">
-        <v>1098224.0</v>
+        <v>927831.0</v>
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="9"/>
@@ -7378,13 +7381,13 @@
       </c>
       <c r="Q19" s="9"/>
       <c r="R19" s="8">
-        <v>1901776.0</v>
+        <v>2072169.0</v>
       </c>
       <c r="S19" s="8">
         <v>3000000.0</v>
       </c>
       <c r="T19" s="8">
-        <v>1651369.0</v>
+        <v>1640862.0</v>
       </c>
       <c r="U19" s="8">
         <v>750000.0</v>
@@ -7415,22 +7418,22 @@
       </c>
       <c r="AD19" s="9"/>
       <c r="AE19" s="8">
-        <v>-155569.0</v>
+        <v>-145062.0</v>
       </c>
       <c r="AF19" s="8">
-        <v>-318142.0</v>
+        <v>-307635.0</v>
       </c>
       <c r="AG19" s="9">
-        <v>0.36607466666667</v>
+        <v>0.309277</v>
       </c>
       <c r="AH19" s="8">
-        <v>-151369.0</v>
+        <v>-140862.0</v>
       </c>
       <c r="AI19" s="8">
-        <v>-756845.0</v>
+        <v>-704310.0</v>
       </c>
       <c r="AJ19" s="8">
-        <v>-12966.0</v>
+        <v>-12066.0</v>
       </c>
       <c r="AK19" s="8"/>
       <c r="AL19" s="9"/>
@@ -7458,19 +7461,19 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1">
-        <v>143527.0</v>
+        <v>121259.0</v>
       </c>
       <c r="J20" s="2">
         <v>0.01</v>
       </c>
       <c r="K20" s="1">
-        <v>10982.0</v>
+        <v>9278.0</v>
       </c>
       <c r="L20" s="1">
-        <v>192545.0</v>
+        <v>261980.0</v>
       </c>
       <c r="M20" s="1">
-        <v>905679.0</v>
+        <v>665851.0</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="2"/>
@@ -7479,13 +7482,13 @@
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>2094321.0</v>
+        <v>2334149.0</v>
       </c>
       <c r="S20" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T20" s="1">
-        <v>1794896.0</v>
+        <v>1762121.0</v>
       </c>
       <c r="U20" s="6">
         <v>750000.0</v>
@@ -7516,22 +7519,22 @@
       </c>
       <c r="AD20" s="2"/>
       <c r="AE20" s="1">
-        <v>-147727.0</v>
+        <v>-125459.0</v>
       </c>
       <c r="AF20" s="1">
-        <v>-465869.0</v>
+        <v>-433094.0</v>
       </c>
       <c r="AG20" s="2">
-        <v>0.301893</v>
+        <v>0.22195033333333</v>
       </c>
       <c r="AH20" s="1">
-        <v>-143527.0</v>
+        <v>-121259.0</v>
       </c>
       <c r="AI20" s="1">
-        <v>-717635.0</v>
+        <v>-606295.0</v>
       </c>
       <c r="AJ20" s="1">
-        <v>-10982.0</v>
+        <v>-9278.0</v>
       </c>
       <c r="AK20" s="1"/>
       <c r="AL20" s="2"/>
@@ -7559,19 +7562,19 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1">
-        <v>134610.0</v>
+        <v>98964.0</v>
       </c>
       <c r="J21" s="2">
         <v>0.01</v>
       </c>
       <c r="K21" s="1">
-        <v>9057.0</v>
+        <v>6659.0</v>
       </c>
       <c r="L21" s="1">
-        <v>185553.0</v>
+        <v>242306.0</v>
       </c>
       <c r="M21" s="1">
-        <v>720127.0</v>
+        <v>423545.0</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="2"/>
@@ -7580,13 +7583,13 @@
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="1">
-        <v>2279873.0</v>
+        <v>2576455.0</v>
       </c>
       <c r="S21" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T21" s="1">
-        <v>1929506.0</v>
+        <v>1861085.0</v>
       </c>
       <c r="U21" s="6">
         <v>750000.0</v>
@@ -7617,22 +7620,22 @@
       </c>
       <c r="AD21" s="2"/>
       <c r="AE21" s="1">
-        <v>-138810.0</v>
+        <v>-103164.0</v>
       </c>
       <c r="AF21" s="1">
-        <v>-604679.0</v>
+        <v>-536258.0</v>
       </c>
       <c r="AG21" s="2">
-        <v>0.24004233333333</v>
+        <v>0.14118166666667</v>
       </c>
       <c r="AH21" s="1">
-        <v>-134610.0</v>
+        <v>-98964.0</v>
       </c>
       <c r="AI21" s="1">
-        <v>-673050.0</v>
+        <v>-494820.0</v>
       </c>
       <c r="AJ21" s="1">
-        <v>-9057.0</v>
+        <v>-6659.0</v>
       </c>
       <c r="AK21" s="1"/>
       <c r="AL21" s="2"/>
@@ -7660,19 +7663,19 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1">
-        <v>124257.0</v>
+        <v>73082.0</v>
       </c>
       <c r="J22" s="2">
         <v>0.01</v>
       </c>
       <c r="K22" s="1">
-        <v>7201.0</v>
+        <v>4235.0</v>
       </c>
       <c r="L22" s="1">
-        <v>177055.0</v>
+        <v>218847.0</v>
       </c>
       <c r="M22" s="1">
-        <v>543071.0</v>
+        <v>204699.0</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="2"/>
@@ -7681,13 +7684,13 @@
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="1">
-        <v>2456929.0</v>
+        <v>2795301.0</v>
       </c>
       <c r="S22" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T22" s="1">
-        <v>2053763.0</v>
+        <v>1934167.0</v>
       </c>
       <c r="U22" s="6">
         <v>750000.0</v>
@@ -7718,22 +7721,22 @@
       </c>
       <c r="AD22" s="2"/>
       <c r="AE22" s="1">
-        <v>-128457.0</v>
+        <v>-77282.0</v>
       </c>
       <c r="AF22" s="1">
-        <v>-733136.0</v>
+        <v>-613540.0</v>
       </c>
       <c r="AG22" s="2">
-        <v>0.18102366666667</v>
+        <v>0.068233</v>
       </c>
       <c r="AH22" s="1">
-        <v>-124257.0</v>
+        <v>-73082.0</v>
       </c>
       <c r="AI22" s="1">
-        <v>-621285.0</v>
+        <v>-365410.0</v>
       </c>
       <c r="AJ22" s="1">
-        <v>-7201.0</v>
+        <v>-4235.0</v>
       </c>
       <c r="AK22" s="1"/>
       <c r="AL22" s="2"/>
@@ -7761,19 +7764,19 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1">
-        <v>111894.0</v>
+        <v>42176.0</v>
       </c>
       <c r="J23" s="2">
         <v>0.01</v>
       </c>
       <c r="K23" s="1">
-        <v>5431.0</v>
+        <v>2047.0</v>
       </c>
       <c r="L23" s="1">
-        <v>166464.0</v>
+        <v>190129.0</v>
       </c>
       <c r="M23" s="1">
-        <v>376608.0</v>
+        <v>14569.0</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="2"/>
@@ -7782,13 +7785,13 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="1">
-        <v>2623392.0</v>
+        <v>2985431.0</v>
       </c>
       <c r="S23" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T23" s="1">
-        <v>2165657.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U23" s="6">
         <v>750000.0</v>
@@ -7819,22 +7822,22 @@
       </c>
       <c r="AD23" s="2"/>
       <c r="AE23" s="1">
-        <v>-116094.0</v>
+        <v>-46376.0</v>
       </c>
       <c r="AF23" s="1">
-        <v>-849230.0</v>
+        <v>-659916.0</v>
       </c>
       <c r="AG23" s="2">
-        <v>0.125536</v>
+        <v>0.0048563333333333</v>
       </c>
       <c r="AH23" s="1">
-        <v>-111894.0</v>
+        <v>-42176.0</v>
       </c>
       <c r="AI23" s="1">
-        <v>-559470.0</v>
+        <v>-210880.0</v>
       </c>
       <c r="AJ23" s="1">
-        <v>-5431.0</v>
+        <v>-2047.0</v>
       </c>
       <c r="AK23" s="1"/>
       <c r="AL23" s="2"/>
@@ -7861,21 +7864,11 @@
         <v>0.0</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="1">
-        <v>96517.0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="K24" s="1">
-        <v>3766.0</v>
-      </c>
-      <c r="L24" s="1">
-        <v>152751.0</v>
-      </c>
-      <c r="M24" s="1">
-        <v>223856.0</v>
-      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="2"/>
       <c r="P24" s="6">
@@ -7883,13 +7876,13 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="1">
-        <v>2776144.0</v>
+        <v>3000000.0</v>
       </c>
       <c r="S24" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T24" s="1">
-        <v>2262174.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U24" s="6">
         <v>750000.0</v>
@@ -7920,27 +7913,25 @@
       </c>
       <c r="AD24" s="2"/>
       <c r="AE24" s="1">
-        <v>-100717.0</v>
+        <v>-4200.0</v>
       </c>
       <c r="AF24" s="1">
-        <v>-949947.0</v>
-      </c>
-      <c r="AG24" s="2">
-        <v>0.074618666666667</v>
-      </c>
+        <v>-664116.0</v>
+      </c>
+      <c r="AG24" s="2"/>
       <c r="AH24" s="1">
-        <v>-96517.0</v>
+        <v>0.0</v>
       </c>
       <c r="AI24" s="1">
-        <v>-482585.0</v>
+        <v>0.0</v>
       </c>
       <c r="AJ24" s="1">
-        <v>-3766.0</v>
+        <v>0.0</v>
       </c>
       <c r="AK24" s="1"/>
       <c r="AL24" s="2"/>
       <c r="AM24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:39">
@@ -7962,21 +7953,11 @@
         <v>0.0</v>
       </c>
       <c r="H25" s="2"/>
-      <c r="I25" s="1">
-        <v>76116.0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="K25" s="1">
-        <v>2239.0</v>
-      </c>
-      <c r="L25" s="1">
-        <v>133878.0</v>
-      </c>
-      <c r="M25" s="1">
-        <v>89979.0</v>
-      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="2"/>
       <c r="P25" s="6">
@@ -7984,13 +7965,13 @@
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="1">
-        <v>2910021.0</v>
+        <v>3000000.0</v>
       </c>
       <c r="S25" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T25" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U25" s="6">
         <v>750000.0</v>
@@ -8021,27 +8002,25 @@
       </c>
       <c r="AD25" s="2"/>
       <c r="AE25" s="1">
-        <v>-80316.0</v>
+        <v>-4200.0</v>
       </c>
       <c r="AF25" s="1">
-        <v>-1030263.0</v>
-      </c>
-      <c r="AG25" s="2">
-        <v>0.029993</v>
-      </c>
+        <v>-668316.0</v>
+      </c>
+      <c r="AG25" s="2"/>
       <c r="AH25" s="1">
-        <v>-76116.0</v>
+        <v>0.0</v>
       </c>
       <c r="AI25" s="1">
-        <v>-380580.0</v>
+        <v>0.0</v>
       </c>
       <c r="AJ25" s="1">
-        <v>-2239.0</v>
+        <v>0.0</v>
       </c>
       <c r="AK25" s="1"/>
       <c r="AL25" s="2"/>
       <c r="AM25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:39">
@@ -8081,7 +8060,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T26" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U26" s="6">
         <v>750000.0</v>
@@ -8115,7 +8094,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF26" s="1">
-        <v>-1034463.0</v>
+        <v>-672516.0</v>
       </c>
       <c r="AG26" s="2"/>
       <c r="AH26" s="1">
@@ -8130,7 +8109,7 @@
       <c r="AK26" s="1"/>
       <c r="AL26" s="2"/>
       <c r="AM26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:39">
@@ -8170,7 +8149,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T27" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U27" s="6">
         <v>750000.0</v>
@@ -8204,7 +8183,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF27" s="1">
-        <v>-1038663.0</v>
+        <v>-676716.0</v>
       </c>
       <c r="AG27" s="2"/>
       <c r="AH27" s="1">
@@ -8219,7 +8198,7 @@
       <c r="AK27" s="1"/>
       <c r="AL27" s="2"/>
       <c r="AM27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:39">
@@ -8259,7 +8238,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T28" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U28" s="6">
         <v>750000.0</v>
@@ -8293,7 +8272,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF28" s="1">
-        <v>-1042863.0</v>
+        <v>-680916.0</v>
       </c>
       <c r="AG28" s="2"/>
       <c r="AH28" s="1">
@@ -8308,7 +8287,7 @@
       <c r="AK28" s="1"/>
       <c r="AL28" s="2"/>
       <c r="AM28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:39">
@@ -8348,7 +8327,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T29" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U29" s="6">
         <v>750000.0</v>
@@ -8382,7 +8361,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF29" s="1">
-        <v>-1047063.0</v>
+        <v>-685116.0</v>
       </c>
       <c r="AG29" s="2"/>
       <c r="AH29" s="1">
@@ -8397,7 +8376,7 @@
       <c r="AK29" s="1"/>
       <c r="AL29" s="2"/>
       <c r="AM29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:39">
@@ -8437,7 +8416,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T30" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U30" s="6">
         <v>750000.0</v>
@@ -8471,7 +8450,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF30" s="1">
-        <v>-1051263.0</v>
+        <v>-689316.0</v>
       </c>
       <c r="AG30" s="2"/>
       <c r="AH30" s="1">
@@ -8486,7 +8465,7 @@
       <c r="AK30" s="1"/>
       <c r="AL30" s="2"/>
       <c r="AM30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:39">
@@ -8526,7 +8505,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T31" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U31" s="6">
         <v>750000.0</v>
@@ -8560,7 +8539,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF31" s="1">
-        <v>-1055463.0</v>
+        <v>-693516.0</v>
       </c>
       <c r="AG31" s="2"/>
       <c r="AH31" s="1">
@@ -8575,7 +8554,7 @@
       <c r="AK31" s="1"/>
       <c r="AL31" s="2"/>
       <c r="AM31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:39">
@@ -8615,7 +8594,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T32" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U32" s="6">
         <v>750000.0</v>
@@ -8649,7 +8628,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF32" s="1">
-        <v>-1059663.0</v>
+        <v>-697716.0</v>
       </c>
       <c r="AG32" s="2"/>
       <c r="AH32" s="1">
@@ -8664,7 +8643,7 @@
       <c r="AK32" s="1"/>
       <c r="AL32" s="2"/>
       <c r="AM32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:39">
@@ -8704,7 +8683,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T33" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U33" s="6">
         <v>750000.0</v>
@@ -8738,7 +8717,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF33" s="1">
-        <v>-1063863.0</v>
+        <v>-701916.0</v>
       </c>
       <c r="AG33" s="2"/>
       <c r="AH33" s="1">
@@ -8753,7 +8732,7 @@
       <c r="AK33" s="1"/>
       <c r="AL33" s="2"/>
       <c r="AM33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:39">
@@ -8793,7 +8772,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T34" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U34" s="6">
         <v>750000.0</v>
@@ -8827,7 +8806,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF34" s="1">
-        <v>-1068063.0</v>
+        <v>-706116.0</v>
       </c>
       <c r="AG34" s="2"/>
       <c r="AH34" s="1">
@@ -8842,7 +8821,7 @@
       <c r="AK34" s="1"/>
       <c r="AL34" s="2"/>
       <c r="AM34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:39">
@@ -8882,7 +8861,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T35" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U35" s="6">
         <v>750000.0</v>
@@ -8916,7 +8895,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF35" s="1">
-        <v>-1072263.0</v>
+        <v>-710316.0</v>
       </c>
       <c r="AG35" s="2"/>
       <c r="AH35" s="1">
@@ -8931,7 +8910,7 @@
       <c r="AK35" s="1"/>
       <c r="AL35" s="2"/>
       <c r="AM35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:39">
@@ -8971,7 +8950,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T36" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U36" s="6">
         <v>750000.0</v>
@@ -9005,7 +8984,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF36" s="1">
-        <v>-1076463.0</v>
+        <v>-714516.0</v>
       </c>
       <c r="AG36" s="2"/>
       <c r="AH36" s="1">
@@ -9020,7 +8999,7 @@
       <c r="AK36" s="1"/>
       <c r="AL36" s="2"/>
       <c r="AM36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:39">
@@ -9060,7 +9039,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T37" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U37" s="6">
         <v>750000.0</v>
@@ -9094,7 +9073,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF37" s="1">
-        <v>-1080663.0</v>
+        <v>-718716.0</v>
       </c>
       <c r="AG37" s="2"/>
       <c r="AH37" s="1">
@@ -9109,7 +9088,7 @@
       <c r="AK37" s="1"/>
       <c r="AL37" s="2"/>
       <c r="AM37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:39">
@@ -9149,7 +9128,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T38" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U38" s="6">
         <v>750000.0</v>
@@ -9183,7 +9162,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF38" s="1">
-        <v>-1084863.0</v>
+        <v>-722916.0</v>
       </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1">
@@ -9198,7 +9177,7 @@
       <c r="AK38" s="1"/>
       <c r="AL38" s="2"/>
       <c r="AM38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:39">
@@ -9238,7 +9217,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T39" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U39" s="6">
         <v>750000.0</v>
@@ -9272,7 +9251,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF39" s="1">
-        <v>-1089063.0</v>
+        <v>-727116.0</v>
       </c>
       <c r="AG39" s="2"/>
       <c r="AH39" s="1">
@@ -9287,7 +9266,7 @@
       <c r="AK39" s="1"/>
       <c r="AL39" s="2"/>
       <c r="AM39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:39">
@@ -9327,7 +9306,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T40" s="11">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U40" s="11">
         <v>750000.0</v>
@@ -9361,7 +9340,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF40" s="11">
-        <v>-1093263.0</v>
+        <v>-731316.0</v>
       </c>
       <c r="AG40" s="12"/>
       <c r="AH40" s="11">
@@ -9376,7 +9355,7 @@
       <c r="AK40" s="11"/>
       <c r="AL40" s="12"/>
       <c r="AM40" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:39">
@@ -9416,7 +9395,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T41" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U41" s="6">
         <v>750000.0</v>
@@ -9450,7 +9429,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF41" s="1">
-        <v>-1097463.0</v>
+        <v>-735516.0</v>
       </c>
       <c r="AG41" s="2"/>
       <c r="AH41" s="1">
@@ -9465,7 +9444,7 @@
       <c r="AK41" s="1"/>
       <c r="AL41" s="2"/>
       <c r="AM41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:39">
@@ -9505,7 +9484,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T42" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U42" s="6">
         <v>750000.0</v>
@@ -9539,7 +9518,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF42" s="1">
-        <v>-1101663.0</v>
+        <v>-739716.0</v>
       </c>
       <c r="AG42" s="2"/>
       <c r="AH42" s="1">
@@ -9554,7 +9533,7 @@
       <c r="AK42" s="1"/>
       <c r="AL42" s="2"/>
       <c r="AM42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:39">
@@ -9594,7 +9573,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T43" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U43" s="6">
         <v>750000.0</v>
@@ -9628,7 +9607,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF43" s="1">
-        <v>-1105863.0</v>
+        <v>-743916.0</v>
       </c>
       <c r="AG43" s="2"/>
       <c r="AH43" s="1">
@@ -9643,7 +9622,7 @@
       <c r="AK43" s="1"/>
       <c r="AL43" s="2"/>
       <c r="AM43" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:39">
@@ -9683,7 +9662,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T44" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U44" s="6">
         <v>750000.0</v>
@@ -9717,7 +9696,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF44" s="1">
-        <v>-1110063.0</v>
+        <v>-748116.0</v>
       </c>
       <c r="AG44" s="2"/>
       <c r="AH44" s="1">
@@ -9732,7 +9711,7 @@
       <c r="AK44" s="1"/>
       <c r="AL44" s="2"/>
       <c r="AM44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:39">
@@ -9772,7 +9751,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T45" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U45" s="6">
         <v>750000.0</v>
@@ -9806,7 +9785,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF45" s="1">
-        <v>-1114263.0</v>
+        <v>-752316.0</v>
       </c>
       <c r="AG45" s="2"/>
       <c r="AH45" s="1">
@@ -9821,7 +9800,7 @@
       <c r="AK45" s="1"/>
       <c r="AL45" s="2"/>
       <c r="AM45" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:39">
@@ -9861,7 +9840,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T46" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U46" s="6">
         <v>750000.0</v>
@@ -9895,7 +9874,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF46" s="1">
-        <v>-1118463.0</v>
+        <v>-756516.0</v>
       </c>
       <c r="AG46" s="2"/>
       <c r="AH46" s="1">
@@ -9910,7 +9889,7 @@
       <c r="AK46" s="1"/>
       <c r="AL46" s="2"/>
       <c r="AM46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:39">
@@ -9950,7 +9929,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T47" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U47" s="6">
         <v>750000.0</v>
@@ -9984,7 +9963,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF47" s="1">
-        <v>-1122663.0</v>
+        <v>-760716.0</v>
       </c>
       <c r="AG47" s="2"/>
       <c r="AH47" s="1">
@@ -9999,7 +9978,7 @@
       <c r="AK47" s="1"/>
       <c r="AL47" s="2"/>
       <c r="AM47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:39">
@@ -10039,7 +10018,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T48" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U48" s="6">
         <v>750000.0</v>
@@ -10073,7 +10052,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF48" s="1">
-        <v>-1126863.0</v>
+        <v>-764916.0</v>
       </c>
       <c r="AG48" s="2"/>
       <c r="AH48" s="1">
@@ -10088,7 +10067,7 @@
       <c r="AK48" s="1"/>
       <c r="AL48" s="2"/>
       <c r="AM48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:39">
@@ -10128,7 +10107,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T49" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U49" s="6">
         <v>750000.0</v>
@@ -10162,7 +10141,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF49" s="1">
-        <v>-1131063.0</v>
+        <v>-769116.0</v>
       </c>
       <c r="AG49" s="2"/>
       <c r="AH49" s="1">
@@ -10177,7 +10156,7 @@
       <c r="AK49" s="1"/>
       <c r="AL49" s="2"/>
       <c r="AM49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:39">
@@ -10217,7 +10196,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T50" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U50" s="6">
         <v>750000.0</v>
@@ -10251,7 +10230,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF50" s="1">
-        <v>-1135263.0</v>
+        <v>-773316.0</v>
       </c>
       <c r="AG50" s="2"/>
       <c r="AH50" s="1">
@@ -10266,7 +10245,7 @@
       <c r="AK50" s="1"/>
       <c r="AL50" s="2"/>
       <c r="AM50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:39">
@@ -10306,7 +10285,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T51" s="1">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U51" s="6">
         <v>750000.0</v>
@@ -10340,7 +10319,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF51" s="1">
-        <v>-1139463.0</v>
+        <v>-777516.0</v>
       </c>
       <c r="AG51" s="2"/>
       <c r="AH51" s="1">
@@ -10355,7 +10334,7 @@
       <c r="AK51" s="1"/>
       <c r="AL51" s="2"/>
       <c r="AM51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:39">
@@ -10395,7 +10374,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T52" s="5">
-        <v>2338290.0</v>
+        <v>1976343.0</v>
       </c>
       <c r="U52" s="5">
         <v>750000.0</v>
@@ -10429,7 +10408,7 @@
         <v>-4200.0</v>
       </c>
       <c r="AF52" s="5">
-        <v>-1143663.0</v>
+        <v>-781716.0</v>
       </c>
       <c r="AG52" s="16"/>
       <c r="AH52" s="5">
@@ -10444,7 +10423,7 @@
       <c r="AK52" s="5"/>
       <c r="AL52" s="16"/>
       <c r="AM52" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:39">
@@ -11577,7 +11556,7 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>